<commit_message>
Commit cuando lo corrimos con  20 LSTMS y 10 dense units, 50 epochs
</commit_message>
<xml_diff>
--- a/run_log/run_results/train_history/training_history_run_0.xlsx
+++ b/run_log/run_results/train_history/training_history_run_0.xlsx
@@ -395,702 +395,702 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>0.04693975299596786</v>
+        <v>0.1685543805360794</v>
       </c>
       <c r="B2">
-        <v>0.9904237389564514</v>
+        <v>0.9514577984809875</v>
       </c>
       <c r="C2">
-        <v>0.06284512579441071</v>
+        <v>0.01198538299649954</v>
       </c>
       <c r="D2">
-        <v>0.9971833229064941</v>
+        <v>0.9987359642982483</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>0.006104138679802418</v>
+        <v>0.05668577179312706</v>
       </c>
       <c r="B3">
-        <v>0.9984574913978577</v>
+        <v>0.9885275363922119</v>
       </c>
       <c r="C3">
-        <v>0.01461739651858807</v>
+        <v>0.003683493472635746</v>
       </c>
       <c r="D3">
-        <v>0.9988140463829041</v>
+        <v>0.9991783499717712</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>0.001739324652589858</v>
+        <v>0.03427432104945183</v>
       </c>
       <c r="B4">
-        <v>0.9993787407875061</v>
+        <v>0.9928836226463318</v>
       </c>
       <c r="C4">
-        <v>0.002749750856310129</v>
+        <v>0.001357663189992309</v>
       </c>
       <c r="D4">
-        <v>0.9994811415672302</v>
+        <v>0.9994943737983704</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>0.001274969661608338</v>
+        <v>0.02565275318920612</v>
       </c>
       <c r="B5">
-        <v>0.9996786713600159</v>
+        <v>0.9932286739349365</v>
       </c>
       <c r="C5">
-        <v>0.002048818627372384</v>
+        <v>0.001237227465026081</v>
       </c>
       <c r="D5">
-        <v>0.999777615070343</v>
+        <v>0.9994943737983704</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
-        <v>0.0006806920864619315</v>
+        <v>0.01652182638645172</v>
       </c>
       <c r="B6">
-        <v>0.9997214674949646</v>
+        <v>0.9966143369674683</v>
       </c>
       <c r="C6">
-        <v>0.05073975026607513</v>
+        <v>0.001224466715939343</v>
       </c>
       <c r="D6">
-        <v>0.9781335592269897</v>
+        <v>0.9994943737983704</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
-        <v>0.0005922017735429108</v>
+        <v>0.01606627926230431</v>
       </c>
       <c r="B7">
-        <v>0.9998500347137451</v>
+        <v>0.9965065121650696</v>
       </c>
       <c r="C7">
-        <v>0.001455631339922547</v>
+        <v>0.00120731454808265</v>
       </c>
       <c r="D7">
-        <v>0.999777615070343</v>
+        <v>0.9994943737983704</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>0.000928357127122581</v>
+        <v>0.01491070538759232</v>
       </c>
       <c r="B8">
-        <v>0.9997429251670837</v>
+        <v>0.9967653155326843</v>
       </c>
       <c r="C8">
-        <v>0.001274107140488923</v>
+        <v>0.0006554255960509181</v>
       </c>
       <c r="D8">
-        <v>0.9998517632484436</v>
+        <v>0.9994943737983704</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
-        <v>0.0003754271601792425</v>
+        <v>0.01238577254116535</v>
       </c>
       <c r="B9">
-        <v>0.9999357461929321</v>
+        <v>0.997218132019043</v>
       </c>
       <c r="C9">
-        <v>0.001578411785885692</v>
+        <v>0.0003809008921962231</v>
       </c>
       <c r="D9">
-        <v>0.9998517632484436</v>
+        <v>0.9998735785484314</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10">
-        <v>0.0001806351210689172</v>
+        <v>0.01169418264180422</v>
       </c>
       <c r="B10">
-        <v>0.9998928904533386</v>
+        <v>0.9971534609794617</v>
       </c>
       <c r="C10">
-        <v>0.001944201881997287</v>
+        <v>0.0006371518829837441</v>
       </c>
       <c r="D10">
-        <v>0.9997035264968872</v>
+        <v>0.9994943737983704</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
-        <v>0.0008072698838077486</v>
+        <v>0.009791713207960129</v>
       </c>
       <c r="B11">
-        <v>0.9997214674949646</v>
+        <v>0.9978435039520264</v>
       </c>
       <c r="C11">
-        <v>0.002302562352269888</v>
+        <v>0.0005319733172655106</v>
       </c>
       <c r="D11">
-        <v>0.9998517632484436</v>
+        <v>0.9994943737983704</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
-        <v>0.0001949363795574754</v>
+        <v>0.008975117467343807</v>
       </c>
       <c r="B12">
-        <v>0.9999571442604065</v>
+        <v>0.9980807304382324</v>
       </c>
       <c r="C12">
-        <v>0.002607382833957672</v>
+        <v>0.0006187378894537687</v>
       </c>
       <c r="D12">
-        <v>0.9998517632484436</v>
+        <v>0.9994943737983704</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13">
-        <v>0.0001879264309536666</v>
+        <v>0.009000315330922604</v>
       </c>
       <c r="B13">
-        <v>0.9999571442604065</v>
+        <v>0.9980160593986511</v>
       </c>
       <c r="C13">
-        <v>0.002298093168064952</v>
+        <v>0.0006525839562527835</v>
       </c>
       <c r="D13">
-        <v>0.9998517632484436</v>
+        <v>0.9994943737983704</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14">
-        <v>0.0003969680401496589</v>
+        <v>0.008788539096713066</v>
       </c>
       <c r="B14">
-        <v>0.9998714327812195</v>
+        <v>0.9980160593986511</v>
       </c>
       <c r="C14">
-        <v>0.00196205428801477</v>
+        <v>0.0004736995324492455</v>
       </c>
       <c r="D14">
-        <v>0.9998517632484436</v>
+        <v>0.9994943737983704</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15">
-        <v>0.0004740967124234885</v>
+        <v>0.007557388860732317</v>
       </c>
       <c r="B15">
-        <v>0.9998928904533386</v>
+        <v>0.9984904527664185</v>
       </c>
       <c r="C15">
-        <v>0.002399453893303871</v>
+        <v>0.0004759454459417611</v>
       </c>
       <c r="D15">
-        <v>0.9998517632484436</v>
+        <v>0.9994943737983704</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16">
-        <v>0.0004843028727918863</v>
+        <v>0.007149933371692896</v>
       </c>
       <c r="B16">
-        <v>0.9998928904533386</v>
+        <v>0.9985336065292358</v>
       </c>
       <c r="C16">
-        <v>0.002007061615586281</v>
+        <v>0.0003978715976700187</v>
       </c>
       <c r="D16">
-        <v>0.9998517632484436</v>
+        <v>0.9994943737983704</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17">
-        <v>8.341002831002697E-05</v>
+        <v>0.008431801572442055</v>
       </c>
       <c r="B17">
-        <v>0.9999571442604065</v>
+        <v>0.9982532858848572</v>
       </c>
       <c r="C17">
-        <v>0.001801385777071118</v>
+        <v>0.0004011470009572804</v>
       </c>
       <c r="D17">
-        <v>0.9998517632484436</v>
+        <v>0.9994943737983704</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18">
-        <v>0.0001336821442237124</v>
+        <v>0.007538223639130592</v>
       </c>
       <c r="B18">
-        <v>0.999914288520813</v>
+        <v>0.9984473586082458</v>
       </c>
       <c r="C18">
-        <v>0.002051786286756396</v>
+        <v>0.0003688928845804185</v>
       </c>
       <c r="D18">
-        <v>0.9998517632484436</v>
+        <v>0.9998735785484314</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19">
-        <v>0.0003709954035002738</v>
+        <v>0.007409240584820509</v>
       </c>
       <c r="B19">
-        <v>0.9998928904533386</v>
+        <v>0.9987276792526245</v>
       </c>
       <c r="C19">
-        <v>0.004172497428953648</v>
+        <v>0.0003067189536523074</v>
       </c>
       <c r="D19">
-        <v>0.9998517632484436</v>
+        <v>0.9999368190765381</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20">
-        <v>4.823507333640009E-05</v>
+        <v>0.007439374923706055</v>
       </c>
       <c r="B20">
-        <v>0.9999786019325256</v>
+        <v>0.9985767006874084</v>
       </c>
       <c r="C20">
-        <v>0.003957303706556559</v>
+        <v>0.0004118172801099718</v>
       </c>
       <c r="D20">
-        <v>0.9998517632484436</v>
+        <v>0.999620795249939</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21">
-        <v>0.0001029425038723275</v>
+        <v>0.007145338226109743</v>
       </c>
       <c r="B21">
-        <v>0.9999357461929321</v>
+        <v>0.9985982775688171</v>
       </c>
       <c r="C21">
-        <v>0.004061858169734478</v>
+        <v>0.0003451149677857757</v>
       </c>
       <c r="D21">
-        <v>0.9998517632484436</v>
+        <v>0.9999368190765381</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22">
-        <v>0.0001373276609228924</v>
+        <v>0.008178493939340115</v>
       </c>
       <c r="B22">
-        <v>0.9999571442604065</v>
+        <v>0.9984688758850098</v>
       </c>
       <c r="C22">
-        <v>0.002880776766687632</v>
+        <v>0.0002993031812366098</v>
       </c>
       <c r="D22">
-        <v>0.9998517632484436</v>
+        <v>0.9999368190765381</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23">
-        <v>0.0002921152045018971</v>
+        <v>0.009255361743271351</v>
       </c>
       <c r="B23">
-        <v>0.9999571442604065</v>
+        <v>0.9982532858848572</v>
       </c>
       <c r="C23">
-        <v>0.003148596966639161</v>
+        <v>0.0002953959046863019</v>
       </c>
       <c r="D23">
-        <v>0.9998517632484436</v>
+        <v>0.9999368190765381</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24">
-        <v>0.0002923418651334941</v>
+        <v>0.007924159988760948</v>
       </c>
       <c r="B24">
-        <v>0.999914288520813</v>
+        <v>0.9984257817268372</v>
       </c>
       <c r="C24">
-        <v>0.004636058583855629</v>
+        <v>0.0002573285310063511</v>
       </c>
       <c r="D24">
-        <v>0.9998517632484436</v>
+        <v>0.9999368190765381</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25">
-        <v>0.0006742379046045244</v>
+        <v>0.006933571305125952</v>
       </c>
       <c r="B25">
-        <v>0.9998286366462708</v>
+        <v>0.9985982775688171</v>
       </c>
       <c r="C25">
-        <v>0.004790619481354952</v>
+        <v>0.0002971312787849456</v>
       </c>
       <c r="D25">
-        <v>0.9998517632484436</v>
+        <v>0.9999368190765381</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26">
-        <v>0.0002228445810033008</v>
+        <v>0.007368875201791525</v>
       </c>
       <c r="B26">
-        <v>0.9999571442604065</v>
+        <v>0.9984904527664185</v>
       </c>
       <c r="C26">
-        <v>0.00416578259319067</v>
+        <v>0.0001980973029276356</v>
       </c>
       <c r="D26">
-        <v>0.9998517632484436</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27">
-        <v>3.189895141986199E-05</v>
+        <v>0.007783030159771442</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>0.9985336065292358</v>
       </c>
       <c r="C27">
-        <v>0.004706538282334805</v>
+        <v>0.0002116225368808955</v>
       </c>
       <c r="D27">
-        <v>0.9998517632484436</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28">
-        <v>2.967343971249647E-05</v>
+        <v>0.007282840553671122</v>
       </c>
       <c r="B28">
-        <v>0.9999786019325256</v>
+        <v>0.9986198544502258</v>
       </c>
       <c r="C28">
-        <v>0.004180197138339281</v>
+        <v>0.0003015203110408038</v>
       </c>
       <c r="D28">
-        <v>0.9998517632484436</v>
+        <v>0.9998735785484314</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29">
-        <v>1.839870151343348E-06</v>
+        <v>0.007369357626885176</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>0.9985120296478271</v>
       </c>
       <c r="C29">
-        <v>0.004079524893313646</v>
+        <v>0.0002253529528388754</v>
       </c>
       <c r="D29">
-        <v>0.9998517632484436</v>
+        <v>0.9999368190765381</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30">
-        <v>2.900073241107748E-06</v>
+        <v>0.0076838294044137</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>0.9985767006874084</v>
       </c>
       <c r="C30">
-        <v>0.003493191208690405</v>
+        <v>0.0003962049377150834</v>
       </c>
       <c r="D30">
-        <v>0.9998517632484436</v>
+        <v>0.9999368190765381</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31">
-        <v>0.0007415831205435097</v>
+        <v>0.006201847456395626</v>
       </c>
       <c r="B31">
-        <v>0.9998714327812195</v>
+        <v>0.9989001750946045</v>
       </c>
       <c r="C31">
-        <v>0.003864601952955127</v>
+        <v>0.0001463020307710394</v>
       </c>
       <c r="D31">
-        <v>0.9998517632484436</v>
+        <v>0.9999368190765381</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32">
-        <v>0.0003805093874689192</v>
+        <v>0.007554376497864723</v>
       </c>
       <c r="B32">
-        <v>0.9999571442604065</v>
+        <v>0.9984688758850098</v>
       </c>
       <c r="C32">
-        <v>0.003861942095682025</v>
+        <v>0.0002316518366569653</v>
       </c>
       <c r="D32">
-        <v>0.9998517632484436</v>
+        <v>0.9999368190765381</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33">
-        <v>3.867033228743821E-05</v>
+        <v>0.008164077065885067</v>
       </c>
       <c r="B33">
-        <v>0.9999786019325256</v>
+        <v>0.9984473586082458</v>
       </c>
       <c r="C33">
-        <v>0.003694018581882119</v>
+        <v>0.0002044559660134837</v>
       </c>
       <c r="D33">
-        <v>0.9998517632484436</v>
+        <v>0.9999368190765381</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34">
-        <v>0.000278520688880235</v>
+        <v>0.007789433002471924</v>
       </c>
       <c r="B34">
-        <v>0.9999357461929321</v>
+        <v>0.9984473586082458</v>
       </c>
       <c r="C34">
-        <v>0.004011130426079035</v>
+        <v>0.0001904767705127597</v>
       </c>
       <c r="D34">
-        <v>0.9998517632484436</v>
+        <v>0.9999368190765381</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35">
-        <v>2.112403490173165E-05</v>
+        <v>0.006942082196474075</v>
       </c>
       <c r="B35">
-        <v>0.9999786019325256</v>
+        <v>0.9985982775688171</v>
       </c>
       <c r="C35">
-        <v>0.00391755485907197</v>
+        <v>0.0001555290655232966</v>
       </c>
       <c r="D35">
-        <v>0.9998517632484436</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36">
-        <v>0.0007736452389508486</v>
+        <v>0.006255006417632103</v>
       </c>
       <c r="B36">
-        <v>0.9998928904533386</v>
+        <v>0.9987923502922058</v>
       </c>
       <c r="C36">
-        <v>0.004887741524726152</v>
+        <v>0.0001506775297457352</v>
       </c>
       <c r="D36">
-        <v>0.9998517632484436</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37">
-        <v>0.0003310273168608546</v>
+        <v>0.006362416781485081</v>
       </c>
       <c r="B37">
-        <v>0.999914288520813</v>
+        <v>0.9986845254898071</v>
       </c>
       <c r="C37">
-        <v>0.004155841656029224</v>
+        <v>0.000153501721797511</v>
       </c>
       <c r="D37">
-        <v>0.9998517632484436</v>
+        <v>0.9999368190765381</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38">
-        <v>0.0002489862381480634</v>
+        <v>0.007286135107278824</v>
       </c>
       <c r="B38">
-        <v>0.9999357461929321</v>
+        <v>0.9985982775688171</v>
       </c>
       <c r="C38">
-        <v>0.003487438894808292</v>
+        <v>0.0002799557114485651</v>
       </c>
       <c r="D38">
-        <v>0.9998517632484436</v>
+        <v>0.9999368190765381</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39">
-        <v>0.0001789374946383759</v>
+        <v>0.007281627040356398</v>
       </c>
       <c r="B39">
-        <v>0.9999357461929321</v>
+        <v>0.9986198544502258</v>
       </c>
       <c r="C39">
-        <v>0.003850506851449609</v>
+        <v>0.0002107537002302706</v>
       </c>
       <c r="D39">
-        <v>0.9998517632484436</v>
+        <v>0.9999368190765381</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40">
-        <v>6.418453267542645E-05</v>
+        <v>0.007905551232397556</v>
       </c>
       <c r="B40">
-        <v>0.9999786019325256</v>
+        <v>0.9984688758850098</v>
       </c>
       <c r="C40">
-        <v>0.004220481030642986</v>
+        <v>0.0001422477071173489</v>
       </c>
       <c r="D40">
-        <v>0.9998517632484436</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41">
-        <v>0.0004181483236607164</v>
+        <v>0.006917495746165514</v>
       </c>
       <c r="B41">
-        <v>0.9998928904533386</v>
+        <v>0.9985767006874084</v>
       </c>
       <c r="C41">
-        <v>0.004438447766005993</v>
+        <v>0.0001651209458941594</v>
       </c>
       <c r="D41">
-        <v>0.9998517632484436</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42">
-        <v>9.726429652801016E-07</v>
+        <v>0.00666859420016408</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>0.9986414313316345</v>
       </c>
       <c r="C42">
-        <v>0.004556612577289343</v>
+        <v>0.000148038103361614</v>
       </c>
       <c r="D42">
-        <v>0.9998517632484436</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43">
-        <v>0.000178697329829447</v>
+        <v>0.006477537099272013</v>
       </c>
       <c r="B43">
-        <v>0.9999786019325256</v>
+        <v>0.9986414313316345</v>
       </c>
       <c r="C43">
-        <v>0.004329185001552105</v>
+        <v>0.0001918048219522461</v>
       </c>
       <c r="D43">
-        <v>0.999777615070343</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44">
-        <v>6.267148273764178E-05</v>
+        <v>0.009205807000398636</v>
       </c>
       <c r="B44">
-        <v>0.9999571442604065</v>
+        <v>0.9983395338058472</v>
       </c>
       <c r="C44">
-        <v>0.006178076844662428</v>
+        <v>0.0001872269494924694</v>
       </c>
       <c r="D44">
-        <v>0.9997035264968872</v>
+        <v>0.9999368190765381</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45">
-        <v>3.062650876017869E-06</v>
+        <v>0.007009216118603945</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>0.9986414313316345</v>
       </c>
       <c r="C45">
-        <v>0.006466618273407221</v>
+        <v>0.0001148005758295767</v>
       </c>
       <c r="D45">
-        <v>0.9998517632484436</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46">
-        <v>7.33243505237624E-05</v>
+        <v>0.007330498192459345</v>
       </c>
       <c r="B46">
-        <v>0.9999786019325256</v>
+        <v>0.9985120296478271</v>
       </c>
       <c r="C46">
-        <v>0.006004385650157928</v>
+        <v>0.0001330219383817166</v>
       </c>
       <c r="D46">
-        <v>0.9998517632484436</v>
+        <v>0.9999368190765381</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47">
-        <v>0.0001872545981314033</v>
+        <v>0.006888146977871656</v>
       </c>
       <c r="B47">
-        <v>0.999914288520813</v>
+        <v>0.9985551834106445</v>
       </c>
       <c r="C47">
-        <v>0.005932081956416368</v>
+        <v>0.0001357696455670521</v>
       </c>
       <c r="D47">
-        <v>0.9998517632484436</v>
+        <v>0.9999368190765381</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48">
-        <v>9.920726006384939E-05</v>
+        <v>0.007587114814668894</v>
       </c>
       <c r="B48">
-        <v>0.9999786019325256</v>
+        <v>0.9984904527664185</v>
       </c>
       <c r="C48">
-        <v>0.005114149767905474</v>
+        <v>0.0001083463721442968</v>
       </c>
       <c r="D48">
-        <v>0.9998517632484436</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49">
-        <v>0.0001161022883024998</v>
+        <v>0.006127714645117521</v>
       </c>
       <c r="B49">
-        <v>0.9999786019325256</v>
+        <v>0.9987276792526245</v>
       </c>
       <c r="C49">
-        <v>0.005511578638106585</v>
+        <v>0.0001025825113174506</v>
       </c>
       <c r="D49">
-        <v>0.9998517632484436</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50">
-        <v>1.066421464201994E-05</v>
+        <v>0.006919529289007187</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>0.9985982775688171</v>
       </c>
       <c r="C50">
-        <v>0.005241688806563616</v>
+        <v>9.808960749069229E-05</v>
       </c>
       <c r="D50">
-        <v>0.9998517632484436</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51">
-        <v>0.0001189765025628731</v>
+        <v>0.007372591178864241</v>
       </c>
       <c r="B51">
-        <v>0.9999571442604065</v>
+        <v>0.9984688758850098</v>
       </c>
       <c r="C51">
-        <v>0.004873020108789206</v>
+        <v>0.0001248484913958237</v>
       </c>
       <c r="D51">
-        <v>0.9998517632484436</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit para red con 20 lstms y 50 dense units
</commit_message>
<xml_diff>
--- a/run_log/run_results/train_history/training_history_run_0.xlsx
+++ b/run_log/run_results/train_history/training_history_run_0.xlsx
@@ -395,702 +395,702 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>0.1685543805360794</v>
+        <v>0.07894483953714371</v>
       </c>
       <c r="B2">
-        <v>0.9514577984809875</v>
+        <v>0.9850173592567444</v>
       </c>
       <c r="C2">
-        <v>0.01198538299649954</v>
+        <v>0.05501991137862206</v>
       </c>
       <c r="D2">
-        <v>0.9987359642982483</v>
+        <v>0.9816839694976807</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>0.05668577179312706</v>
+        <v>0.01143994275480509</v>
       </c>
       <c r="B3">
-        <v>0.9885275363922119</v>
+        <v>0.9979863166809082</v>
       </c>
       <c r="C3">
-        <v>0.003683493472635746</v>
+        <v>0.01424783375114202</v>
       </c>
       <c r="D3">
-        <v>0.9991783499717712</v>
+        <v>0.9985420107841492</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>0.03427432104945183</v>
+        <v>0.007136783096939325</v>
       </c>
       <c r="B4">
-        <v>0.9928836226463318</v>
+        <v>0.9982260465621948</v>
       </c>
       <c r="C4">
-        <v>0.001357663189992309</v>
+        <v>0.03617475926876068</v>
       </c>
       <c r="D4">
-        <v>0.9994943737983704</v>
+        <v>0.9897029399871826</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>0.02565275318920612</v>
+        <v>0.003146222559735179</v>
       </c>
       <c r="B5">
-        <v>0.9932286739349365</v>
+        <v>0.9989931583404541</v>
       </c>
       <c r="C5">
-        <v>0.001237227465026081</v>
+        <v>0.006303617730736732</v>
       </c>
       <c r="D5">
-        <v>0.9994943737983704</v>
+        <v>0.9990887641906738</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
-        <v>0.01652182638645172</v>
+        <v>0.002033980097621679</v>
       </c>
       <c r="B6">
-        <v>0.9966143369674683</v>
+        <v>0.9993767142295837</v>
       </c>
       <c r="C6">
-        <v>0.001224466715939343</v>
+        <v>0.002838238375261426</v>
       </c>
       <c r="D6">
-        <v>0.9994943737983704</v>
+        <v>0.9993621110916138</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
-        <v>0.01606627926230431</v>
+        <v>0.001335583976469934</v>
       </c>
       <c r="B7">
-        <v>0.9965065121650696</v>
+        <v>0.9996164441108704</v>
       </c>
       <c r="C7">
-        <v>0.00120731454808265</v>
+        <v>0.00534950103610754</v>
       </c>
       <c r="D7">
-        <v>0.9994943737983704</v>
+        <v>0.9991798996925354</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>0.01491070538759232</v>
+        <v>0.001106253708712757</v>
       </c>
       <c r="B8">
-        <v>0.9967653155326843</v>
+        <v>0.999712347984314</v>
       </c>
       <c r="C8">
-        <v>0.0006554255960509181</v>
+        <v>0.00417760806158185</v>
       </c>
       <c r="D8">
-        <v>0.9994943737983704</v>
+        <v>0.9993621110916138</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
-        <v>0.01238577254116535</v>
+        <v>0.0004791124956682324</v>
       </c>
       <c r="B9">
-        <v>0.997218132019043</v>
+        <v>0.999856173992157</v>
       </c>
       <c r="C9">
-        <v>0.0003809008921962231</v>
+        <v>0.003315480891615152</v>
       </c>
       <c r="D9">
-        <v>0.9998735785484314</v>
+        <v>0.9996355175971985</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10">
-        <v>0.01169418264180422</v>
+        <v>0.0008339165942743421</v>
       </c>
       <c r="B10">
-        <v>0.9971534609794617</v>
+        <v>0.9997602701187134</v>
       </c>
       <c r="C10">
-        <v>0.0006371518829837441</v>
+        <v>0.02276963368058205</v>
       </c>
       <c r="D10">
-        <v>0.9994943737983704</v>
+        <v>0.9953526258468628</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
-        <v>0.009791713207960129</v>
+        <v>0.001345777069218457</v>
       </c>
       <c r="B11">
-        <v>0.9978435039520264</v>
+        <v>0.999712347984314</v>
       </c>
       <c r="C11">
-        <v>0.0005319733172655106</v>
+        <v>0.002359997713938355</v>
       </c>
       <c r="D11">
-        <v>0.9994943737983704</v>
+        <v>0.9997266530990601</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
-        <v>0.008975117467343807</v>
+        <v>0.0004446671810001135</v>
       </c>
       <c r="B12">
-        <v>0.9980807304382324</v>
+        <v>0.9998082518577576</v>
       </c>
       <c r="C12">
-        <v>0.0006187378894537687</v>
+        <v>0.003632189007475972</v>
       </c>
       <c r="D12">
-        <v>0.9994943737983704</v>
+        <v>0.9997266530990601</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13">
-        <v>0.009000315330922604</v>
+        <v>0.0004180538235232234</v>
       </c>
       <c r="B13">
-        <v>0.9980160593986511</v>
+        <v>0.9998082518577576</v>
       </c>
       <c r="C13">
-        <v>0.0006525839562527835</v>
+        <v>0.003190836403518915</v>
       </c>
       <c r="D13">
-        <v>0.9994943737983704</v>
+        <v>0.9998177289962769</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14">
-        <v>0.008788539096713066</v>
+        <v>0.00107716559432447</v>
       </c>
       <c r="B14">
-        <v>0.9980160593986511</v>
+        <v>0.999712347984314</v>
       </c>
       <c r="C14">
-        <v>0.0004736995324492455</v>
+        <v>0.003981982823461294</v>
       </c>
       <c r="D14">
-        <v>0.9994943737983704</v>
+        <v>0.9995443820953369</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15">
-        <v>0.007557388860732317</v>
+        <v>0.0004904359811916947</v>
       </c>
       <c r="B15">
-        <v>0.9984904527664185</v>
+        <v>0.9999280571937561</v>
       </c>
       <c r="C15">
-        <v>0.0004759454459417611</v>
+        <v>0.003341034520417452</v>
       </c>
       <c r="D15">
-        <v>0.9994943737983704</v>
+        <v>0.9998177289962769</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16">
-        <v>0.007149933371692896</v>
+        <v>0.000872167176567018</v>
       </c>
       <c r="B16">
-        <v>0.9985336065292358</v>
+        <v>0.9999040961265564</v>
       </c>
       <c r="C16">
-        <v>0.0003978715976700187</v>
+        <v>0.005824651103466749</v>
       </c>
       <c r="D16">
-        <v>0.9994943737983704</v>
+        <v>0.9989976286888123</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17">
-        <v>0.008431801572442055</v>
+        <v>0.0006204347591847181</v>
       </c>
       <c r="B17">
-        <v>0.9982532858848572</v>
+        <v>0.9998801350593567</v>
       </c>
       <c r="C17">
-        <v>0.0004011470009572804</v>
+        <v>0.004680939950048923</v>
       </c>
       <c r="D17">
-        <v>0.9994943737983704</v>
+        <v>0.9994532465934753</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18">
-        <v>0.007538223639130592</v>
+        <v>0.000323024665703997</v>
       </c>
       <c r="B18">
-        <v>0.9984473586082458</v>
+        <v>0.9999040961265564</v>
       </c>
       <c r="C18">
-        <v>0.0003688928845804185</v>
+        <v>0.003417379222810268</v>
       </c>
       <c r="D18">
-        <v>0.9998735785484314</v>
+        <v>0.9997266530990601</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19">
-        <v>0.007409240584820509</v>
+        <v>0.0004191637272015214</v>
       </c>
       <c r="B19">
-        <v>0.9987276792526245</v>
+        <v>0.9999280571937561</v>
       </c>
       <c r="C19">
-        <v>0.0003067189536523074</v>
+        <v>0.00300374673679471</v>
       </c>
       <c r="D19">
-        <v>0.9999368190765381</v>
+        <v>0.9995443820953369</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20">
-        <v>0.007439374923706055</v>
+        <v>0.0005814707255922258</v>
       </c>
       <c r="B20">
-        <v>0.9985767006874084</v>
+        <v>0.9998801350593567</v>
       </c>
       <c r="C20">
-        <v>0.0004118172801099718</v>
+        <v>0.002603017725050449</v>
       </c>
       <c r="D20">
-        <v>0.999620795249939</v>
+        <v>0.9998177289962769</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21">
-        <v>0.007145338226109743</v>
+        <v>0.0001891005813376978</v>
       </c>
       <c r="B21">
-        <v>0.9985982775688171</v>
+        <v>0.9999520778656006</v>
       </c>
       <c r="C21">
-        <v>0.0003451149677857757</v>
+        <v>0.003995790611952543</v>
       </c>
       <c r="D21">
-        <v>0.9999368190765381</v>
+        <v>0.9996355175971985</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22">
-        <v>0.008178493939340115</v>
+        <v>7.626674050698057E-05</v>
       </c>
       <c r="B22">
-        <v>0.9984688758850098</v>
+        <v>0.9999760389328003</v>
       </c>
       <c r="C22">
-        <v>0.0002993031812366098</v>
+        <v>0.004770407453179359</v>
       </c>
       <c r="D22">
-        <v>0.9999368190765381</v>
+        <v>0.9997266530990601</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23">
-        <v>0.009255361743271351</v>
+        <v>0.0007936455658636987</v>
       </c>
       <c r="B23">
-        <v>0.9982532858848572</v>
+        <v>0.999856173992157</v>
       </c>
       <c r="C23">
-        <v>0.0002953959046863019</v>
+        <v>0.003464552341029048</v>
       </c>
       <c r="D23">
-        <v>0.9999368190765381</v>
+        <v>0.9997266530990601</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24">
-        <v>0.007924159988760948</v>
+        <v>0.0003479622828308493</v>
       </c>
       <c r="B24">
-        <v>0.9984257817268372</v>
+        <v>0.9999280571937561</v>
       </c>
       <c r="C24">
-        <v>0.0002573285310063511</v>
+        <v>0.003709803801029921</v>
       </c>
       <c r="D24">
-        <v>0.9999368190765381</v>
+        <v>0.9997266530990601</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25">
-        <v>0.006933571305125952</v>
+        <v>4.396321310196072E-05</v>
       </c>
       <c r="B25">
-        <v>0.9985982775688171</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>0.0002971312787849456</v>
+        <v>0.00415083346888423</v>
       </c>
       <c r="D25">
-        <v>0.9999368190765381</v>
+        <v>0.9997266530990601</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26">
-        <v>0.007368875201791525</v>
+        <v>2.971356479974929E-05</v>
       </c>
       <c r="B26">
-        <v>0.9984904527664185</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>0.0001980973029276356</v>
+        <v>0.00397802796214819</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0.9997266530990601</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27">
-        <v>0.007783030159771442</v>
+        <v>0.001085724332369864</v>
       </c>
       <c r="B27">
-        <v>0.9985336065292358</v>
+        <v>0.999856173992157</v>
       </c>
       <c r="C27">
-        <v>0.0002116225368808955</v>
+        <v>0.006191342603415251</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0.9994532465934753</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28">
-        <v>0.007282840553671122</v>
+        <v>0.0008579105488024652</v>
       </c>
       <c r="B28">
-        <v>0.9986198544502258</v>
+        <v>0.9998082518577576</v>
       </c>
       <c r="C28">
-        <v>0.0003015203110408038</v>
+        <v>0.004604802466928959</v>
       </c>
       <c r="D28">
-        <v>0.9998735785484314</v>
+        <v>0.9997266530990601</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29">
-        <v>0.007369357626885176</v>
+        <v>0.0002173398970626295</v>
       </c>
       <c r="B29">
-        <v>0.9985120296478271</v>
+        <v>0.9999040961265564</v>
       </c>
       <c r="C29">
-        <v>0.0002253529528388754</v>
+        <v>0.005196835845708847</v>
       </c>
       <c r="D29">
-        <v>0.9999368190765381</v>
+        <v>0.9997266530990601</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30">
-        <v>0.0076838294044137</v>
+        <v>0.0002047561574727297</v>
       </c>
       <c r="B30">
-        <v>0.9985767006874084</v>
+        <v>0.9999760389328003</v>
       </c>
       <c r="C30">
-        <v>0.0003962049377150834</v>
+        <v>0.005126964300870895</v>
       </c>
       <c r="D30">
-        <v>0.9999368190765381</v>
+        <v>0.9998177289962769</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31">
-        <v>0.006201847456395626</v>
+        <v>5.552189395530149E-05</v>
       </c>
       <c r="B31">
-        <v>0.9989001750946045</v>
+        <v>0.9999760389328003</v>
       </c>
       <c r="C31">
-        <v>0.0001463020307710394</v>
+        <v>0.005708858370780945</v>
       </c>
       <c r="D31">
-        <v>0.9999368190765381</v>
+        <v>0.9996355175971985</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32">
-        <v>0.007554376497864723</v>
+        <v>0.0001251735957339406</v>
       </c>
       <c r="B32">
-        <v>0.9984688758850098</v>
+        <v>0.9999520778656006</v>
       </c>
       <c r="C32">
-        <v>0.0002316518366569653</v>
+        <v>0.005812831688672304</v>
       </c>
       <c r="D32">
-        <v>0.9999368190765381</v>
+        <v>0.9997266530990601</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33">
-        <v>0.008164077065885067</v>
+        <v>0.000203552728635259</v>
       </c>
       <c r="B33">
-        <v>0.9984473586082458</v>
+        <v>0.9999280571937561</v>
       </c>
       <c r="C33">
-        <v>0.0002044559660134837</v>
+        <v>0.005553629249334335</v>
       </c>
       <c r="D33">
-        <v>0.9999368190765381</v>
+        <v>0.9995443820953369</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34">
-        <v>0.007789433002471924</v>
+        <v>0.0001581512478878722</v>
       </c>
       <c r="B34">
-        <v>0.9984473586082458</v>
+        <v>0.9999280571937561</v>
       </c>
       <c r="C34">
-        <v>0.0001904767705127597</v>
+        <v>0.00608416274189949</v>
       </c>
       <c r="D34">
-        <v>0.9999368190765381</v>
+        <v>0.9996355175971985</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35">
-        <v>0.006942082196474075</v>
+        <v>3.100594767602161E-05</v>
       </c>
       <c r="B35">
-        <v>0.9985982775688171</v>
+        <v>1</v>
       </c>
       <c r="C35">
-        <v>0.0001555290655232966</v>
+        <v>0.006395941600203514</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>0.9997266530990601</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36">
-        <v>0.006255006417632103</v>
+        <v>0.00104407430626452</v>
       </c>
       <c r="B36">
-        <v>0.9987923502922058</v>
+        <v>0.9998082518577576</v>
       </c>
       <c r="C36">
-        <v>0.0001506775297457352</v>
+        <v>0.006021083332598209</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>0.9996355175971985</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37">
-        <v>0.006362416781485081</v>
+        <v>0.0003287571016699076</v>
       </c>
       <c r="B37">
-        <v>0.9986845254898071</v>
+        <v>0.9999040961265564</v>
       </c>
       <c r="C37">
-        <v>0.000153501721797511</v>
+        <v>0.002093495801091194</v>
       </c>
       <c r="D37">
-        <v>0.9999368190765381</v>
+        <v>0.9997266530990601</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38">
-        <v>0.007286135107278824</v>
+        <v>8.474537025904283E-05</v>
       </c>
       <c r="B38">
-        <v>0.9985982775688171</v>
+        <v>0.9999760389328003</v>
       </c>
       <c r="C38">
-        <v>0.0002799557114485651</v>
+        <v>0.003535917494446039</v>
       </c>
       <c r="D38">
-        <v>0.9999368190765381</v>
+        <v>0.9997266530990601</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39">
-        <v>0.007281627040356398</v>
+        <v>1.38871037052013E-05</v>
       </c>
       <c r="B39">
-        <v>0.9986198544502258</v>
+        <v>1</v>
       </c>
       <c r="C39">
-        <v>0.0002107537002302706</v>
+        <v>0.003172539873048663</v>
       </c>
       <c r="D39">
-        <v>0.9999368190765381</v>
+        <v>0.9997266530990601</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40">
-        <v>0.007905551232397556</v>
+        <v>2.678169403225183E-05</v>
       </c>
       <c r="B40">
-        <v>0.9984688758850098</v>
+        <v>1</v>
       </c>
       <c r="C40">
-        <v>0.0001422477071173489</v>
+        <v>0.002246905118227005</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>0.9997266530990601</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41">
-        <v>0.006917495746165514</v>
+        <v>0.0003182807995472103</v>
       </c>
       <c r="B41">
-        <v>0.9985767006874084</v>
+        <v>0.9999040961265564</v>
       </c>
       <c r="C41">
-        <v>0.0001651209458941594</v>
+        <v>0.004259370267391205</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>0.9998177289962769</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42">
-        <v>0.00666859420016408</v>
+        <v>0.0004242907161824405</v>
       </c>
       <c r="B42">
-        <v>0.9986414313316345</v>
+        <v>0.9999280571937561</v>
       </c>
       <c r="C42">
-        <v>0.000148038103361614</v>
+        <v>0.004586369264870882</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>0.9997266530990601</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43">
-        <v>0.006477537099272013</v>
+        <v>0.000241204776102677</v>
       </c>
       <c r="B43">
-        <v>0.9986414313316345</v>
+        <v>0.9999280571937561</v>
       </c>
       <c r="C43">
-        <v>0.0001918048219522461</v>
+        <v>0.003723932662978768</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>0.9998177289962769</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44">
-        <v>0.009205807000398636</v>
+        <v>4.509017890086398E-05</v>
       </c>
       <c r="B44">
-        <v>0.9983395338058472</v>
+        <v>1</v>
       </c>
       <c r="C44">
-        <v>0.0001872269494924694</v>
+        <v>0.004271246958523989</v>
       </c>
       <c r="D44">
-        <v>0.9999368190765381</v>
+        <v>0.9998177289962769</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45">
-        <v>0.007009216118603945</v>
+        <v>0.0001570691674714908</v>
       </c>
       <c r="B45">
-        <v>0.9986414313316345</v>
+        <v>0.9999520778656006</v>
       </c>
       <c r="C45">
-        <v>0.0001148005758295767</v>
+        <v>0.003537895390763879</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>0.9998177289962769</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46">
-        <v>0.007330498192459345</v>
+        <v>6.044161636964418E-05</v>
       </c>
       <c r="B46">
-        <v>0.9985120296478271</v>
+        <v>0.9999760389328003</v>
       </c>
       <c r="C46">
-        <v>0.0001330219383817166</v>
+        <v>0.001979353139176965</v>
       </c>
       <c r="D46">
-        <v>0.9999368190765381</v>
+        <v>0.9998177289962769</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47">
-        <v>0.006888146977871656</v>
+        <v>0.0005082806455902755</v>
       </c>
       <c r="B47">
-        <v>0.9985551834106445</v>
+        <v>0.9999280571937561</v>
       </c>
       <c r="C47">
-        <v>0.0001357696455670521</v>
+        <v>0.004723383579403162</v>
       </c>
       <c r="D47">
-        <v>0.9999368190765381</v>
+        <v>0.9997266530990601</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48">
-        <v>0.007587114814668894</v>
+        <v>0.002066576387733221</v>
       </c>
       <c r="B48">
-        <v>0.9984904527664185</v>
+        <v>0.9996883869171143</v>
       </c>
       <c r="C48">
-        <v>0.0001083463721442968</v>
+        <v>0.003528243629261851</v>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>0.9996355175971985</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49">
-        <v>0.006127714645117521</v>
+        <v>8.175086259143427E-05</v>
       </c>
       <c r="B49">
-        <v>0.9987276792526245</v>
+        <v>1</v>
       </c>
       <c r="C49">
-        <v>0.0001025825113174506</v>
+        <v>0.003408631077036262</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>0.9996355175971985</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50">
-        <v>0.006919529289007187</v>
+        <v>7.30858082533814E-05</v>
       </c>
       <c r="B50">
-        <v>0.9985982775688171</v>
+        <v>0.9999520778656006</v>
       </c>
       <c r="C50">
-        <v>9.808960749069229E-05</v>
+        <v>0.003614519257098436</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>0.9996355175971985</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51">
-        <v>0.007372591178864241</v>
+        <v>3.423586895223707E-05</v>
       </c>
       <c r="B51">
-        <v>0.9984688758850098</v>
+        <v>0.9999760389328003</v>
       </c>
       <c r="C51">
-        <v>0.0001248484913958237</v>
+        <v>0.004889555741101503</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>0.9997266530990601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit con 128 capas densas, 20 lstm y 50 epochs, 0.5 de dropout
</commit_message>
<xml_diff>
--- a/run_log/run_results/train_history/training_history_run_0.xlsx
+++ b/run_log/run_results/train_history/training_history_run_0.xlsx
@@ -395,702 +395,702 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>0.07894483953714371</v>
+        <v>0.06282870471477509</v>
       </c>
       <c r="B2">
-        <v>0.9850173592567444</v>
+        <v>0.9828430414199829</v>
       </c>
       <c r="C2">
-        <v>0.05501991137862206</v>
+        <v>0.01085071451961994</v>
       </c>
       <c r="D2">
-        <v>0.9816839694976807</v>
+        <v>0.9979230165481567</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>0.01143994275480509</v>
+        <v>0.01039525680243969</v>
       </c>
       <c r="B3">
-        <v>0.9979863166809082</v>
+        <v>0.9982308149337769</v>
       </c>
       <c r="C3">
-        <v>0.01424783375114202</v>
+        <v>0.00875630509108305</v>
       </c>
       <c r="D3">
-        <v>0.9985420107841492</v>
+        <v>0.9979230165481567</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>0.007136783096939325</v>
+        <v>0.007095101289451122</v>
       </c>
       <c r="B4">
-        <v>0.9982260465621948</v>
+        <v>0.998457133769989</v>
       </c>
       <c r="C4">
-        <v>0.03617475926876068</v>
+        <v>0.005982016678899527</v>
       </c>
       <c r="D4">
-        <v>0.9897029399871826</v>
+        <v>0.99806147813797</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>0.003146222559735179</v>
+        <v>0.003250523470342159</v>
       </c>
       <c r="B5">
-        <v>0.9989931583404541</v>
+        <v>0.9989919662475586</v>
       </c>
       <c r="C5">
-        <v>0.006303617730736732</v>
+        <v>0.001100260997191072</v>
       </c>
       <c r="D5">
-        <v>0.9990887641906738</v>
+        <v>0.9993076920509338</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
-        <v>0.002033980097621679</v>
+        <v>0.002281023422256112</v>
       </c>
       <c r="B6">
-        <v>0.9993767142295837</v>
+        <v>0.9995062947273254</v>
       </c>
       <c r="C6">
-        <v>0.002838238375261426</v>
+        <v>0.0003513776755426079</v>
       </c>
       <c r="D6">
-        <v>0.9993621110916138</v>
+        <v>0.9998615384101868</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
-        <v>0.001335583976469934</v>
+        <v>0.001272676978260279</v>
       </c>
       <c r="B7">
-        <v>0.9996164441108704</v>
+        <v>0.9996502995491028</v>
       </c>
       <c r="C7">
-        <v>0.00534950103610754</v>
+        <v>0.0008334434824064374</v>
       </c>
       <c r="D7">
-        <v>0.9991798996925354</v>
+        <v>0.9997230768203735</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>0.001106253708712757</v>
+        <v>0.001134548685513437</v>
       </c>
       <c r="B8">
-        <v>0.999712347984314</v>
+        <v>0.9997119903564453</v>
       </c>
       <c r="C8">
-        <v>0.00417760806158185</v>
+        <v>0.0002371456648688763</v>
       </c>
       <c r="D8">
-        <v>0.9993621110916138</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
-        <v>0.0004791124956682324</v>
+        <v>0.0007800249150022864</v>
       </c>
       <c r="B9">
-        <v>0.999856173992157</v>
+        <v>0.9997736811637878</v>
       </c>
       <c r="C9">
-        <v>0.003315480891615152</v>
+        <v>0.0003103387134615332</v>
       </c>
       <c r="D9">
-        <v>0.9996355175971985</v>
+        <v>0.9998615384101868</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10">
-        <v>0.0008339165942743421</v>
+        <v>0.00178591173607856</v>
       </c>
       <c r="B10">
-        <v>0.9997602701187134</v>
+        <v>0.9996502995491028</v>
       </c>
       <c r="C10">
-        <v>0.02276963368058205</v>
+        <v>0.000146520949783735</v>
       </c>
       <c r="D10">
-        <v>0.9953526258468628</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
-        <v>0.001345777069218457</v>
+        <v>0.0008525385637767613</v>
       </c>
       <c r="B11">
-        <v>0.999712347984314</v>
+        <v>0.9996914267539978</v>
       </c>
       <c r="C11">
-        <v>0.002359997713938355</v>
+        <v>0.0001066033728420734</v>
       </c>
       <c r="D11">
-        <v>0.9997266530990601</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
-        <v>0.0004446671810001135</v>
+        <v>0.0007122239330783486</v>
       </c>
       <c r="B12">
-        <v>0.9998082518577576</v>
+        <v>0.9998354315757751</v>
       </c>
       <c r="C12">
-        <v>0.003632189007475972</v>
+        <v>0.0002789738646242768</v>
       </c>
       <c r="D12">
-        <v>0.9997266530990601</v>
+        <v>0.9998615384101868</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13">
-        <v>0.0004180538235232234</v>
+        <v>0.0005686317454092205</v>
       </c>
       <c r="B13">
-        <v>0.9998082518577576</v>
+        <v>0.9998354315757751</v>
       </c>
       <c r="C13">
-        <v>0.003190836403518915</v>
+        <v>3.645956212494639E-06</v>
       </c>
       <c r="D13">
-        <v>0.9998177289962769</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14">
-        <v>0.00107716559432447</v>
+        <v>0.001130313496105373</v>
       </c>
       <c r="B14">
-        <v>0.999712347984314</v>
+        <v>0.9997325539588928</v>
       </c>
       <c r="C14">
-        <v>0.003981982823461294</v>
+        <v>2.455276990076527E-05</v>
       </c>
       <c r="D14">
-        <v>0.9995443820953369</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15">
-        <v>0.0004904359811916947</v>
+        <v>0.0003081322356592864</v>
       </c>
       <c r="B15">
-        <v>0.9999280571937561</v>
+        <v>0.9998765587806702</v>
       </c>
       <c r="C15">
-        <v>0.003341034520417452</v>
+        <v>5.720556146115996E-06</v>
       </c>
       <c r="D15">
-        <v>0.9998177289962769</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16">
-        <v>0.000872167176567018</v>
+        <v>0.0002759694471023977</v>
       </c>
       <c r="B16">
-        <v>0.9999040961265564</v>
+        <v>0.9998765587806702</v>
       </c>
       <c r="C16">
-        <v>0.005824651103466749</v>
+        <v>0.000296323501970619</v>
       </c>
       <c r="D16">
-        <v>0.9989976286888123</v>
+        <v>0.9997230768203735</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17">
-        <v>0.0006204347591847181</v>
+        <v>0.0004831361875403672</v>
       </c>
       <c r="B17">
-        <v>0.9998801350593567</v>
+        <v>0.9999383091926575</v>
       </c>
       <c r="C17">
-        <v>0.004680939950048923</v>
+        <v>2.068367393803783E-06</v>
       </c>
       <c r="D17">
-        <v>0.9994532465934753</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18">
-        <v>0.000323024665703997</v>
+        <v>0.0005349786952137947</v>
       </c>
       <c r="B18">
-        <v>0.9999040961265564</v>
+        <v>0.9998354315757751</v>
       </c>
       <c r="C18">
-        <v>0.003417379222810268</v>
+        <v>0.000638014986179769</v>
       </c>
       <c r="D18">
-        <v>0.9997266530990601</v>
+        <v>0.9997230768203735</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19">
-        <v>0.0004191637272015214</v>
+        <v>0.0005231896648183465</v>
       </c>
       <c r="B19">
-        <v>0.9999280571937561</v>
+        <v>0.9998148679733276</v>
       </c>
       <c r="C19">
-        <v>0.00300374673679471</v>
+        <v>0.00359085900709033</v>
       </c>
       <c r="D19">
-        <v>0.9995443820953369</v>
+        <v>0.9997230768203735</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20">
-        <v>0.0005814707255922258</v>
+        <v>0.0008616555132903159</v>
       </c>
       <c r="B20">
-        <v>0.9998801350593567</v>
+        <v>0.9998354315757751</v>
       </c>
       <c r="C20">
-        <v>0.002603017725050449</v>
+        <v>0.002779387170448899</v>
       </c>
       <c r="D20">
-        <v>0.9998177289962769</v>
+        <v>0.9997230768203735</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21">
-        <v>0.0001891005813376978</v>
+        <v>0.0006011150544509292</v>
       </c>
       <c r="B21">
-        <v>0.9999520778656006</v>
+        <v>0.9998971223831177</v>
       </c>
       <c r="C21">
-        <v>0.003995790611952543</v>
+        <v>1.653091931075323E-05</v>
       </c>
       <c r="D21">
-        <v>0.9996355175971985</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22">
-        <v>7.626674050698057E-05</v>
+        <v>0.0002357810008106753</v>
       </c>
       <c r="B22">
-        <v>0.9999760389328003</v>
+        <v>0.999958872795105</v>
       </c>
       <c r="C22">
-        <v>0.004770407453179359</v>
+        <v>2.828609467542265E-06</v>
       </c>
       <c r="D22">
-        <v>0.9997266530990601</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23">
-        <v>0.0007936455658636987</v>
+        <v>2.041883453784976E-05</v>
       </c>
       <c r="B23">
-        <v>0.999856173992157</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <v>0.003464552341029048</v>
+        <v>1.050290211423999E-05</v>
       </c>
       <c r="D23">
-        <v>0.9997266530990601</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24">
-        <v>0.0003479622828308493</v>
+        <v>0.001388830598443747</v>
       </c>
       <c r="B24">
-        <v>0.9999280571937561</v>
+        <v>0.9998148679733276</v>
       </c>
       <c r="C24">
-        <v>0.003709803801029921</v>
+        <v>2.844104983523721E-06</v>
       </c>
       <c r="D24">
-        <v>0.9997266530990601</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25">
-        <v>4.396321310196072E-05</v>
+        <v>0.000322646606946364</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0.9998765587806702</v>
       </c>
       <c r="C25">
-        <v>0.00415083346888423</v>
+        <v>2.761302084763884E-06</v>
       </c>
       <c r="D25">
-        <v>0.9997266530990601</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26">
-        <v>2.971356479974929E-05</v>
+        <v>0.000334899581503123</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>0.9999383091926575</v>
       </c>
       <c r="C26">
-        <v>0.00397802796214819</v>
+        <v>7.479215855710208E-05</v>
       </c>
       <c r="D26">
-        <v>0.9997266530990601</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27">
-        <v>0.001085724332369864</v>
+        <v>0.0001319392613368109</v>
       </c>
       <c r="B27">
-        <v>0.999856173992157</v>
+        <v>0.999958872795105</v>
       </c>
       <c r="C27">
-        <v>0.006191342603415251</v>
+        <v>4.18257259298116E-05</v>
       </c>
       <c r="D27">
-        <v>0.9994532465934753</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28">
-        <v>0.0008579105488024652</v>
+        <v>6.819709960836917E-05</v>
       </c>
       <c r="B28">
-        <v>0.9998082518577576</v>
+        <v>0.999958872795105</v>
       </c>
       <c r="C28">
-        <v>0.004604802466928959</v>
+        <v>0.0001725208421703428</v>
       </c>
       <c r="D28">
-        <v>0.9997266530990601</v>
+        <v>0.9998615384101868</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29">
-        <v>0.0002173398970626295</v>
+        <v>0.00052812130888924</v>
       </c>
       <c r="B29">
-        <v>0.9999040961265564</v>
+        <v>0.9999176859855652</v>
       </c>
       <c r="C29">
-        <v>0.005196835845708847</v>
+        <v>2.240926960439538E-06</v>
       </c>
       <c r="D29">
-        <v>0.9997266530990601</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30">
-        <v>0.0002047561574727297</v>
+        <v>1.930411781358998E-05</v>
       </c>
       <c r="B30">
-        <v>0.9999760389328003</v>
+        <v>1</v>
       </c>
       <c r="C30">
-        <v>0.005126964300870895</v>
+        <v>7.000030018389225E-05</v>
       </c>
       <c r="D30">
-        <v>0.9998177289962769</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31">
-        <v>5.552189395530149E-05</v>
+        <v>2.858807238226291E-05</v>
       </c>
       <c r="B31">
-        <v>0.9999760389328003</v>
+        <v>0.9999794363975525</v>
       </c>
       <c r="C31">
-        <v>0.005708858370780945</v>
+        <v>6.076084559936135E-07</v>
       </c>
       <c r="D31">
-        <v>0.9996355175971985</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32">
-        <v>0.0001251735957339406</v>
+        <v>0.0001593780471011996</v>
       </c>
       <c r="B32">
-        <v>0.9999520778656006</v>
+        <v>0.999958872795105</v>
       </c>
       <c r="C32">
-        <v>0.005812831688672304</v>
+        <v>0.0004123479302506894</v>
       </c>
       <c r="D32">
-        <v>0.9997266530990601</v>
+        <v>0.9998615384101868</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33">
-        <v>0.000203552728635259</v>
+        <v>0.0009153003338724375</v>
       </c>
       <c r="B33">
-        <v>0.9999280571937561</v>
+        <v>0.9998971223831177</v>
       </c>
       <c r="C33">
-        <v>0.005553629249334335</v>
+        <v>0.0003424502210691571</v>
       </c>
       <c r="D33">
-        <v>0.9995443820953369</v>
+        <v>0.9998615384101868</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34">
-        <v>0.0001581512478878722</v>
+        <v>0.0004767657956108451</v>
       </c>
       <c r="B34">
-        <v>0.9999280571937561</v>
+        <v>0.9999176859855652</v>
       </c>
       <c r="C34">
-        <v>0.00608416274189949</v>
+        <v>1.358641839033226E-06</v>
       </c>
       <c r="D34">
-        <v>0.9996355175971985</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35">
-        <v>3.100594767602161E-05</v>
+        <v>0.0001063353411154822</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>0.999958872795105</v>
       </c>
       <c r="C35">
-        <v>0.006395941600203514</v>
+        <v>1.23450035971473E-07</v>
       </c>
       <c r="D35">
-        <v>0.9997266530990601</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36">
-        <v>0.00104407430626452</v>
+        <v>1.737596721795853E-05</v>
       </c>
       <c r="B36">
-        <v>0.9998082518577576</v>
+        <v>1</v>
       </c>
       <c r="C36">
-        <v>0.006021083332598209</v>
+        <v>1.276242187486787E-06</v>
       </c>
       <c r="D36">
-        <v>0.9996355175971985</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37">
-        <v>0.0003287571016699076</v>
+        <v>0.0003067961079068482</v>
       </c>
       <c r="B37">
-        <v>0.9999040961265564</v>
+        <v>0.9999383091926575</v>
       </c>
       <c r="C37">
-        <v>0.002093495801091194</v>
+        <v>1.210474920299021E-06</v>
       </c>
       <c r="D37">
-        <v>0.9997266530990601</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38">
-        <v>8.474537025904283E-05</v>
+        <v>0.0004406876105349511</v>
       </c>
       <c r="B38">
-        <v>0.9999760389328003</v>
+        <v>0.9998971223831177</v>
       </c>
       <c r="C38">
-        <v>0.003535917494446039</v>
+        <v>9.759023811284351E-08</v>
       </c>
       <c r="D38">
-        <v>0.9997266530990601</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39">
-        <v>1.38871037052013E-05</v>
+        <v>0.0003309159365016967</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>0.999958872795105</v>
       </c>
       <c r="C39">
-        <v>0.003172539873048663</v>
+        <v>4.71189650852466E-07</v>
       </c>
       <c r="D39">
-        <v>0.9997266530990601</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40">
-        <v>2.678169403225183E-05</v>
+        <v>0.0005877171061001718</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>0.9999176859855652</v>
       </c>
       <c r="C40">
-        <v>0.002246905118227005</v>
+        <v>2.990876879493953E-08</v>
       </c>
       <c r="D40">
-        <v>0.9997266530990601</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41">
-        <v>0.0003182807995472103</v>
+        <v>8.043642083066516E-06</v>
       </c>
       <c r="B41">
-        <v>0.9999040961265564</v>
+        <v>1</v>
       </c>
       <c r="C41">
-        <v>0.004259370267391205</v>
+        <v>9.375569653968796E-09</v>
       </c>
       <c r="D41">
-        <v>0.9998177289962769</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42">
-        <v>0.0004242907161824405</v>
+        <v>0.0002470318868290633</v>
       </c>
       <c r="B42">
-        <v>0.9999280571937561</v>
+        <v>0.9999176859855652</v>
       </c>
       <c r="C42">
-        <v>0.004586369264870882</v>
+        <v>8.941028681874741E-06</v>
       </c>
       <c r="D42">
-        <v>0.9997266530990601</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43">
-        <v>0.000241204776102677</v>
+        <v>0.0002659836027305573</v>
       </c>
       <c r="B43">
-        <v>0.9999280571937561</v>
+        <v>0.9998971223831177</v>
       </c>
       <c r="C43">
-        <v>0.003723932662978768</v>
+        <v>0.0009957951260730624</v>
       </c>
       <c r="D43">
-        <v>0.9998177289962769</v>
+        <v>0.9997230768203735</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44">
-        <v>4.509017890086398E-05</v>
+        <v>0.0001214111834997311</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>0.9999794363975525</v>
       </c>
       <c r="C44">
-        <v>0.004271246958523989</v>
+        <v>1.445577709091594E-05</v>
       </c>
       <c r="D44">
-        <v>0.9998177289962769</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45">
-        <v>0.0001570691674714908</v>
+        <v>0.0003123309288639575</v>
       </c>
       <c r="B45">
-        <v>0.9999520778656006</v>
+        <v>0.999958872795105</v>
       </c>
       <c r="C45">
-        <v>0.003537895390763879</v>
+        <v>1.270274879061617E-05</v>
       </c>
       <c r="D45">
-        <v>0.9998177289962769</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46">
-        <v>6.044161636964418E-05</v>
+        <v>0.0003110425022896379</v>
       </c>
       <c r="B46">
-        <v>0.9999760389328003</v>
+        <v>0.9999383091926575</v>
       </c>
       <c r="C46">
-        <v>0.001979353139176965</v>
+        <v>1.616396048120805E-06</v>
       </c>
       <c r="D46">
-        <v>0.9998177289962769</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47">
-        <v>0.0005082806455902755</v>
+        <v>0.0004860930785071105</v>
       </c>
       <c r="B47">
-        <v>0.9999280571937561</v>
+        <v>0.9998765587806702</v>
       </c>
       <c r="C47">
-        <v>0.004723383579403162</v>
+        <v>1.115945224228199E-06</v>
       </c>
       <c r="D47">
-        <v>0.9997266530990601</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48">
-        <v>0.002066576387733221</v>
+        <v>2.635229975567199E-06</v>
       </c>
       <c r="B48">
-        <v>0.9996883869171143</v>
+        <v>1</v>
       </c>
       <c r="C48">
-        <v>0.003528243629261851</v>
+        <v>9.829424243434914E-07</v>
       </c>
       <c r="D48">
-        <v>0.9996355175971985</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49">
-        <v>8.175086259143427E-05</v>
+        <v>0.000124282407341525</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>0.999958872795105</v>
       </c>
       <c r="C49">
-        <v>0.003408631077036262</v>
+        <v>1.333587874796649E-06</v>
       </c>
       <c r="D49">
-        <v>0.9996355175971985</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50">
-        <v>7.30858082533814E-05</v>
+        <v>6.188482802826911E-05</v>
       </c>
       <c r="B50">
-        <v>0.9999520778656006</v>
+        <v>0.9999794363975525</v>
       </c>
       <c r="C50">
-        <v>0.003614519257098436</v>
+        <v>1.006882222043259E-08</v>
       </c>
       <c r="D50">
-        <v>0.9996355175971985</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51">
-        <v>3.423586895223707E-05</v>
+        <v>0.0001330009836237878</v>
       </c>
       <c r="B51">
-        <v>0.9999760389328003</v>
+        <v>0.999958872795105</v>
       </c>
       <c r="C51">
-        <v>0.004889555741101503</v>
+        <v>8.201206583180465E-06</v>
       </c>
       <c r="D51">
-        <v>0.9997266530990601</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>